<commit_message>
add figure for problem statement
</commit_message>
<xml_diff>
--- a/figures/OneThreadCompare.xlsx
+++ b/figures/OneThreadCompare.xlsx
@@ -13,8 +13,10 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Figures" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="15">
   <si>
     <t>CFQ</t>
   </si>
@@ -57,6 +59,18 @@
   </si>
   <si>
     <t>WRITE</t>
+  </si>
+  <si>
+    <t>BM Sequential Read</t>
+  </si>
+  <si>
+    <t>VM Sequential Read</t>
+  </si>
+  <si>
+    <t>BM Sequential Write</t>
+  </si>
+  <si>
+    <t>VM Sequential Write</t>
   </si>
 </sst>
 </file>
@@ -150,6 +164,1224 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
+              <a:t>Bare-metal's and VM's throughput</a:t>
+            </a:r>
+            <a:br>
+              <a:rPr lang="en-US"/>
+            </a:br>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> for sequential read and write (MB/s)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BM Sequential Read</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$28:$C$30</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>CFQ</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Deadline</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Noop</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$28:$D$30</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>101.25615234375</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100.06591796875</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>104.52587890625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-434D-49A2-9E08-AFEF10E48EA6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>VM Sequential Read</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$28:$C$30</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>CFQ</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Deadline</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Noop</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$28:$E$30</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>82.579394531250003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>84.929882812499898</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>84.235742187499895</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-434D-49A2-9E08-AFEF10E48EA6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BM Sequential Write</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$28:$C$30</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>CFQ</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Deadline</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Noop</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$28:$F$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>103.99951171875</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>102.20146484375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>107.4689453125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-434D-49A2-9E08-AFEF10E48EA6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>VM Sequential Write</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$28:$C$30</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>CFQ</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Deadline</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Noop</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$28:$G$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>91.447265625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>91.8828125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>87.683398437500003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-434D-49A2-9E08-AFEF10E48EA6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="604028968"/>
+        <c:axId val="604029296"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="604028968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="604029296"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="604029296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="604028968"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sequential Write</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$21:$C$23</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>CFQ</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Deadline</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Noop</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$21:$D$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>103.99951171875</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>102.20146484375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>107.4689453125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E5EB-4E5A-BD85-D2A4FB0EDC85}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SVM-MT 1C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$21:$C$23</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>CFQ</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Deadline</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Noop</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$21:$E$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>63.9267578125</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>86.897363281249895</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>78.82763671875</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E5EB-4E5A-BD85-D2A4FB0EDC85}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SVM-MT 2C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$21:$C$23</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>CFQ</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Deadline</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Noop</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$21:$F$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>47.345898437499898</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>85.532421874999898</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>73.255859375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-E5EB-4E5A-BD85-D2A4FB0EDC85}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SVM-MT 4C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$21:$C$23</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>CFQ</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Deadline</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Noop</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$21:$G$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>91.447265625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>91.8828125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>87.683398437500003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-E5EB-4E5A-BD85-D2A4FB0EDC85}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SVM-MT 8C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$21:$C$23</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>CFQ</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Deadline</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Noop</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$21:$H$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>78.606542968750006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>75.184179687500006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>85.382421875000006</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-E5EB-4E5A-BD85-D2A4FB0EDC85}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SVM-MT 16C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$21:$C$23</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>CFQ</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Deadline</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Noop</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$21:$I$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>59.761914062499898</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>76.0537109375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>71.112597656250003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-E5EB-4E5A-BD85-D2A4FB0EDC85}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="483674320"/>
+        <c:axId val="483677928"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="483674320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="483677928"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="483677928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="483674320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
               <a:t>Sequential</a:t>
             </a:r>
             <a:r>
@@ -258,7 +1490,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-70E3-42B0-9619-E86FDC3A9EDC}"/>
+              <c16:uniqueId val="{00000000-AF28-47C5-BFC7-5DFA31DCF76B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -323,7 +1555,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-70E3-42B0-9619-E86FDC3A9EDC}"/>
+              <c16:uniqueId val="{00000001-AF28-47C5-BFC7-5DFA31DCF76B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -388,7 +1620,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-70E3-42B0-9619-E86FDC3A9EDC}"/>
+              <c16:uniqueId val="{00000002-AF28-47C5-BFC7-5DFA31DCF76B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -453,7 +1685,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-70E3-42B0-9619-E86FDC3A9EDC}"/>
+              <c16:uniqueId val="{00000003-AF28-47C5-BFC7-5DFA31DCF76B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -518,7 +1750,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-70E3-42B0-9619-E86FDC3A9EDC}"/>
+              <c16:uniqueId val="{00000004-AF28-47C5-BFC7-5DFA31DCF76B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -583,7 +1815,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-70E3-42B0-9619-E86FDC3A9EDC}"/>
+              <c16:uniqueId val="{00000005-AF28-47C5-BFC7-5DFA31DCF76B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -784,670 +2016,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Sequential Write</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$D$20</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>BM</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$C$21:$C$23</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>CFQ</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Deadline</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Noop</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$21:$D$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>103.99951171875</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>102.20146484375</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>107.4689453125</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0498-4128-9F66-EE0475B11B5C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$E$20</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>SVM-MT 1C</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$C$21:$C$23</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>CFQ</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Deadline</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Noop</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$E$21:$E$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>63.9267578125</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>86.897363281249895</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>78.82763671875</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0498-4128-9F66-EE0475B11B5C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$F$20</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>SVM-MT 2C</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$C$21:$C$23</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>CFQ</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Deadline</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Noop</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$F$21:$F$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>47.345898437499898</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>85.532421874999898</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>73.255859375</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-0498-4128-9F66-EE0475B11B5C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$G$20</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>SVM-MT 4C</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$C$21:$C$23</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>CFQ</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Deadline</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Noop</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$G$21:$G$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>91.447265625</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>91.8828125</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>87.683398437500003</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-0498-4128-9F66-EE0475B11B5C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$H$20</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>SVM-MT 8C</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$C$21:$C$23</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>CFQ</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Deadline</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Noop</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$H$21:$H$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>78.606542968750006</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>75.184179687500006</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>85.382421875000006</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-0498-4128-9F66-EE0475B11B5C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$I$20</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>SVM-MT 16C</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent6"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$C$21:$C$23</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>CFQ</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Deadline</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Noop</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$I$21:$I$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>59.761914062499898</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>76.0537109375</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>71.112597656250003</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-0498-4128-9F66-EE0475B11B5C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="483674320"/>
-        <c:axId val="483677928"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="483674320"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="483677928"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="483677928"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="483674320"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1528,6 +2096,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2534,25 +3142,565 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2568,21 +3716,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2862,17 +4012,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C10:I23"/>
+  <dimension ref="C10:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20:I23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" customWidth="1"/>
     <col min="7" max="7" width="18.5703125" customWidth="1"/>
     <col min="8" max="8" width="18.28515625" customWidth="1"/>
     <col min="9" max="9" width="12.7109375" customWidth="1"/>
@@ -3062,9 +4212,166 @@
         <v>71.112597656250003</v>
       </c>
     </row>
+    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1">
+        <v>101.25615234375</v>
+      </c>
+      <c r="E28" s="1">
+        <v>82.579394531250003</v>
+      </c>
+      <c r="F28">
+        <v>103.99951171875</v>
+      </c>
+      <c r="G28">
+        <v>91.447265625</v>
+      </c>
+    </row>
+    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="1">
+        <v>100.06591796875</v>
+      </c>
+      <c r="E29" s="1">
+        <v>84.929882812499898</v>
+      </c>
+      <c r="F29">
+        <v>102.20146484375</v>
+      </c>
+      <c r="G29">
+        <v>91.8828125</v>
+      </c>
+    </row>
+    <row r="30" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="1">
+        <v>104.52587890625</v>
+      </c>
+      <c r="E30" s="1">
+        <v>84.235742187499895</v>
+      </c>
+      <c r="F30">
+        <v>107.4689453125</v>
+      </c>
+      <c r="G30">
+        <v>87.683398437500003</v>
+      </c>
+    </row>
+    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34" s="1">
+        <f>(D28/D28)*100</f>
+        <v>100</v>
+      </c>
+      <c r="E34" s="1">
+        <f>(E28/D28)*100</f>
+        <v>81.554940238006367</v>
+      </c>
+      <c r="F34">
+        <f>(F28/F28)*100</f>
+        <v>100</v>
+      </c>
+      <c r="G34">
+        <v>91.447265625</v>
+      </c>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="1">
+        <f>(D29/D29)*100</f>
+        <v>100</v>
+      </c>
+      <c r="E35" s="1">
+        <f>(E29/D29)*100</f>
+        <v>84.873935638129055</v>
+      </c>
+      <c r="F35">
+        <f>(F29/F29)*100</f>
+        <v>100</v>
+      </c>
+      <c r="G35">
+        <v>91.8828125</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="1">
+        <f>(D30/D30)*100</f>
+        <v>100</v>
+      </c>
+      <c r="E36" s="1">
+        <f>(E30/D30)*100</f>
+        <v>80.588408410372253</v>
+      </c>
+      <c r="F36">
+        <f>(F30/F30)*100</f>
+        <v>100</v>
+      </c>
+      <c r="G36">
+        <v>87.683398437500003</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>